<commit_message>
BIG UPDATE: Authentication is now server-side!
</commit_message>
<xml_diff>
--- a/docs/C_ProjectSchedule.xlsx
+++ b/docs/C_ProjectSchedule.xlsx
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,8 +221,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,8 +262,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -278,14 +291,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -300,9 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -325,9 +351,15 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="4" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,213 +665,259 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="125.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" ht="22.5" customHeight="1">
-      <c r="A2" s="1"/>
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:11" ht="22.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="5" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:11" s="5" customFormat="1" ht="45.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B11" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="5" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="44.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A13" s="15"/>
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A14" s="1"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="5" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="14" t="s">
+    <row r="15" spans="1:11" s="5" customFormat="1" ht="44.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A15" s="15"/>
+      <c r="B15" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" s="5" customFormat="1" ht="115.5">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" s="5" customFormat="1" ht="117" thickTop="1" thickBot="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A17" s="1"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B19" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B21" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="5" customFormat="1">
-      <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="13" t="s">
+    <row r="23" spans="1:11" s="5" customFormat="1" thickTop="1" thickBot="1">
+      <c r="A23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B24" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="1:11" thickTop="1" thickBot="1">
+      <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A26" s="1"/>
+    <row r="26" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B26" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A27" s="1"/>
+    <row r="27" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B27" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A28" s="1"/>
-      <c r="B28" s="12" t="s">
+    <row r="28" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B28" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A29" s="1"/>
-      <c r="B29" s="12" t="s">
+    <row r="29" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B29" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A32" s="1"/>
+    <row r="32" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A33" s="1"/>
+    <row r="33" spans="2:2" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A34" s="1"/>
+    <row r="34" spans="2:2" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+    <row r="35" spans="2:2" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B35" s="16"/>
+    </row>
+    <row r="36" spans="2:2" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B36" s="16"/>
+    </row>
+    <row r="37" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B37" s="16"/>
+    </row>
+    <row r="38" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B38" s="16"/>
+    </row>
+    <row r="39" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B39" s="16"/>
+    </row>
+    <row r="40" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B40" s="16"/>
+    </row>
+    <row r="41" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B41" s="16"/>
+    </row>
+    <row r="42" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B43" s="16"/>
+    </row>
+    <row r="44" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B44" s="16"/>
+    </row>
+    <row r="45" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="2:2" thickTop="1" thickBot="1">
+      <c r="B46" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All changes up to 28 Feb 2025
</commit_message>
<xml_diff>
--- a/docs/C_ProjectSchedule.xlsx
+++ b/docs/C_ProjectSchedule.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Commarian\Documents\SpringbokApp\springbok\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView minimized="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -662,13 +662,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1"/>

</xml_diff>